<commit_message>
turned CPT_Run into a block format
</commit_message>
<xml_diff>
--- a/CPT/CPT_List.xlsx
+++ b/CPT/CPT_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://loyolauniversitychicago-my.sharepoint.com/personal/canlab_luc_edu/Documents/Documents/MATLAB/148_Salience_Stim_Scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://loyolauniversitychicago-my.sharepoint.com/personal/canlab_luc_edu/Documents/Documents/MATLAB/148_Salience_Stim_Scripts/CANLab-Code/CPT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{042044F7-7F40-44CA-999E-21D44B77D3BE}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0410B6FA-3DF7-4A21-8B52-BF81F979BC3F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
   <si>
     <t>A</t>
   </si>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>L</t>
-  </si>
-  <si>
-    <t>E</t>
   </si>
 </sst>
 </file>
@@ -485,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A150"/>
+  <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="E158" sqref="E158"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,507 +737,7 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>